<commit_message>
Arquivo da métrica personalizado
</commit_message>
<xml_diff>
--- a/Documentação/Metrica.xlsx
+++ b/Documentação/Metrica.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaov\Documents\Repositórios Git\ProjetoIndividual\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaov\Documents\Repositórios git\ProjetoIndividual\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D935CB2-57CE-413C-A5FB-9E27D12C8847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53DD8739-6C2C-4271-93F6-91E1A3BE5301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{DB9DC9F7-A836-4053-8176-EC43AF6DF0FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{DB9DC9F7-A836-4053-8176-EC43AF6DF0FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,21 +74,76 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF62C400"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF59FF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB04"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA704"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3209"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -96,16 +151,111 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -114,6 +264,18 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF0000"/>
+      <color rgb="FFFF3209"/>
+      <color rgb="FFFF8000"/>
+      <color rgb="FFFFA704"/>
+      <color rgb="FFFFEB04"/>
+      <color rgb="FF59FF00"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FF62C400"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -425,39 +587,39 @@
   <dimension ref="B2:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="2">
+    <row r="3" spans="2:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
         <v>0</v>
       </c>
       <c r="C3" s="2">
@@ -478,7 +640,7 @@
       <c r="H3" s="2">
         <v>0.9</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="3">
         <v>1</v>
       </c>
     </row>

</xml_diff>